<commit_message>
saving the excel data
</commit_message>
<xml_diff>
--- a/src/assets/template/collection-template.xlsx
+++ b/src/assets/template/collection-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Practice\NFGI\src\assets\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbhinavPandey\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198D6F43-172B-4A62-82DF-F6A8E20E475D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31603EDA-107D-4CB0-9942-1F1475A03BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Total Amount</t>
   </si>
@@ -44,7 +44,10 @@
     <t>Membership_Id</t>
   </si>
   <si>
-    <t>Late_Fees(if_applicable)</t>
+    <t>Loan_Id</t>
+  </si>
+  <si>
+    <t>Late_Fees</t>
   </si>
 </sst>
 </file>
@@ -435,121 +438,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG10"/>
+  <dimension ref="A1:AH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AG1" sqref="AG1"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.59765625" customWidth="1"/>
-    <col min="2" max="2" width="15.296875" customWidth="1"/>
-    <col min="33" max="33" width="24" customWidth="1"/>
+    <col min="1" max="2" width="13.59765625" customWidth="1"/>
+    <col min="3" max="4" width="15.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1">
         <v>1</v>
       </c>
-      <c r="D1" s="1">
+      <c r="F1" s="1">
         <v>2</v>
       </c>
-      <c r="E1" s="1">
+      <c r="G1" s="1">
         <v>3</v>
       </c>
-      <c r="F1" s="1">
+      <c r="H1" s="1">
         <v>4</v>
       </c>
-      <c r="G1" s="1">
+      <c r="I1" s="1">
         <v>5</v>
       </c>
-      <c r="H1" s="1">
+      <c r="J1" s="1">
         <v>6</v>
       </c>
-      <c r="I1" s="1">
+      <c r="K1" s="1">
         <v>7</v>
       </c>
-      <c r="J1" s="1">
+      <c r="L1" s="1">
         <v>8</v>
       </c>
-      <c r="K1" s="1">
+      <c r="M1" s="1">
         <v>9</v>
       </c>
-      <c r="L1" s="1">
+      <c r="N1" s="1">
         <v>10</v>
       </c>
-      <c r="M1" s="1">
+      <c r="O1" s="1">
         <v>11</v>
       </c>
-      <c r="N1" s="1">
+      <c r="P1" s="1">
         <v>12</v>
       </c>
-      <c r="O1" s="1">
+      <c r="Q1" s="1">
         <v>13</v>
       </c>
-      <c r="P1" s="1">
+      <c r="R1" s="1">
         <v>14</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="S1" s="1">
         <v>15</v>
       </c>
-      <c r="R1" s="1">
+      <c r="T1" s="1">
         <v>16</v>
       </c>
-      <c r="S1" s="1">
+      <c r="U1" s="1">
         <v>17</v>
       </c>
-      <c r="T1" s="1">
+      <c r="V1" s="1">
         <v>18</v>
       </c>
-      <c r="U1" s="1">
+      <c r="W1" s="1">
         <v>19</v>
       </c>
-      <c r="V1" s="1">
+      <c r="X1" s="1">
         <v>20</v>
       </c>
-      <c r="W1" s="1">
+      <c r="Y1" s="1">
         <v>21</v>
       </c>
-      <c r="X1" s="1">
+      <c r="Z1" s="1">
         <v>22</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="AA1" s="1">
         <v>23</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="AB1" s="1">
         <v>24</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="AC1" s="1">
         <v>25</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="AD1" s="1">
         <v>26</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="AE1" s="1">
         <v>27</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="AF1" s="1">
         <v>28</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="AG1" s="1">
         <v>29</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="AH1" s="1">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -583,8 +588,9 @@
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -618,8 +624,9 @@
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -653,8 +660,9 @@
       <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -688,8 +696,9 @@
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -723,8 +732,9 @@
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -758,8 +768,9 @@
       <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -793,8 +804,9 @@
       <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -828,22 +840,17 @@
       <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="1">
-        <f t="shared" ref="C10:AG10" si="0">SUM(C2:C9)</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E10:AH10" si="0">SUM(E2:E9)</f>
         <v>0</v>
       </c>
       <c r="F10" s="1">
@@ -955,6 +962,10 @@
         <v>0</v>
       </c>
       <c r="AG10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>